<commit_message>
Add updated MOC data with CSV export
</commit_message>
<xml_diff>
--- a/nozzle-calculations/moc_data.xlsx
+++ b/nozzle-calculations/moc_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Jason\ProjectCaelus\propulsion\nozzle-calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D50067B-C4FA-45D6-B080-2EB12A144DF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD44B1F1-8270-499A-93FF-FC1E4B1B57B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2232" yWindow="2232" windowWidth="17280" windowHeight="8964" xr2:uid="{E71B74F8-B24B-4894-900F-336A06F299E9}"/>
   </bookViews>
@@ -379,100 +379,353 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1872359B-A718-4694-90C5-3B80906C487E}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B11"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>0</v>
       </c>
       <c r="B1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>15.227067222484973</v>
+      </c>
+      <c r="C1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>62.770192169959579</v>
+        <v>22.473693933007748</v>
       </c>
       <c r="B2">
-        <v>64.109227043215327</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>25.199196518943083</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>110.75602347503758</v>
+        <v>29.722275188127529</v>
       </c>
       <c r="B3">
-        <v>87.169868445665898</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>28.295530262795801</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>147.68909072840583</v>
+        <v>34.153532513107017</v>
       </c>
       <c r="B4">
-        <v>101.63611491338393</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>30.079942447862663</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>191.93649555047458</v>
+        <v>38.261896087222766</v>
       </c>
       <c r="B5">
-        <v>116.47349898893634</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>31.668230001666924</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>246.43583582119231</v>
+        <v>42.268384043729085</v>
       </c>
       <c r="B6">
-        <v>131.77797321016203</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>33.153362471893381</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>314.59872273492658</v>
+        <v>46.279251758217093</v>
       </c>
       <c r="B7">
-        <v>147.30651237266579</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+        <v>34.576934123207032</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>400.77999184927563</v>
+        <v>50.357539951497323</v>
       </c>
       <c r="B8">
-        <v>162.47445777336324</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+        <v>35.960820607690735</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>510.7384465455325</v>
+        <v>54.546543300144471</v>
       </c>
       <c r="B9">
-        <v>176.22877853254255</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+        <v>37.317548943874876</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>652.2354093932604</v>
+        <v>58.879476474951218</v>
       </c>
       <c r="B10">
-        <v>186.81319924766245</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+        <v>38.654543003430874</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>835.87955211018641</v>
+        <v>63.384097679175881</v>
       </c>
       <c r="B11">
-        <v>191.38468540146093</v>
+        <v>39.976125065687171</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>68.085177075997294</v>
+      </c>
+      <c r="B12">
+        <v>41.284553754015711</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>73.005936021122082</v>
+      </c>
+      <c r="B13">
+        <v>42.580597778855143</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>78.168952826997582</v>
+      </c>
+      <c r="B14">
+        <v>43.863865204006082</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>83.596774571649362</v>
+      </c>
+      <c r="B15">
+        <v>45.132994077560035</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>89.312359600325365</v>
+      </c>
+      <c r="B16">
+        <v>46.385759120780676</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>95.339419730144414</v>
+      </c>
+      <c r="B17">
+        <v>47.619124318470661</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>101.70270247624951</v>
+      </c>
+      <c r="B18">
+        <v>48.829258371390218</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>108.4282380431073</v>
+      </c>
+      <c r="B19">
+        <v>50.011522909929695</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>115.54356700780011</v>
+      </c>
+      <c r="B20">
+        <v>51.160439299863903</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>123.07795946129629</v>
+      </c>
+      <c r="B21">
+        <v>52.269637413571225</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>131.06263327736957</v>
+      </c>
+      <c r="B22">
+        <v>53.331788182791115</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>139.53097729473504</v>
+      </c>
+      <c r="B23">
+        <v>54.338520709398907</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>148.51878405240365</v>
+      </c>
+      <c r="B24">
+        <v>55.280323974474229</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>158.06449603956796</v>
+      </c>
+      <c r="B25">
+        <v>56.146432628277381</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>168.20946904965939</v>
+      </c>
+      <c r="B26">
+        <v>56.924695889012611</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>178.99825606763144</v>
+      </c>
+      <c r="B27">
+        <v>57.601428178673331</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>190.47891511183616</v>
+      </c>
+      <c r="B28">
+        <v>58.161239748114831</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>202.70334456184622</v>
+      </c>
+      <c r="B29">
+        <v>58.586845168418044</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>215.72764971047636</v>
+      </c>
+      <c r="B30">
+        <v>58.858847174625488</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>229.61254457070822</v>
+      </c>
+      <c r="B31">
+        <v>58.95549292705909</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add updated pipe fluid flow figures
</commit_message>
<xml_diff>
--- a/nozzle-calculations/moc_data.xlsx
+++ b/nozzle-calculations/moc_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Jason\ProjectCaelus\propulsion\nozzle-calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD44B1F1-8270-499A-93FF-FC1E4B1B57B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2755616-7891-47A4-B711-A52F1BCE08F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2232" yWindow="2232" windowWidth="17280" windowHeight="8964" xr2:uid="{E71B74F8-B24B-4894-900F-336A06F299E9}"/>
   </bookViews>
@@ -381,8 +381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1872359B-A718-4694-90C5-3B80906C487E}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -392,7 +392,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>15.227067222484973</v>
+        <v>15.23</v>
       </c>
       <c r="C1">
         <v>0</v>
@@ -400,10 +400,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>22.473693933007748</v>
+        <v>28.630468503753782</v>
       </c>
       <c r="B2">
-        <v>25.199196518943083</v>
+        <v>27.933647815573622</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -411,10 +411,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>29.722275188127529</v>
+        <v>46.424324163695431</v>
       </c>
       <c r="B3">
-        <v>28.295530262795801</v>
+        <v>34.955264023511084</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -422,10 +422,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>34.153532513107017</v>
+        <v>59.220651167493827</v>
       </c>
       <c r="B4">
-        <v>30.079942447862663</v>
+        <v>39.099598143212624</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -433,10 +433,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>38.261896087222766</v>
+        <v>73.521852300752712</v>
       </c>
       <c r="B5">
-        <v>31.668230001666924</v>
+        <v>43.079867294704265</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -444,10 +444,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>42.268384043729085</v>
+        <v>90.011373845611956</v>
       </c>
       <c r="B6">
-        <v>33.153362471893381</v>
+        <v>46.935324028156764</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -455,10 +455,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>46.279251758217093</v>
+        <v>109.33485710037152</v>
       </c>
       <c r="B7">
-        <v>34.576934123207032</v>
+        <v>50.610054172001263</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -466,10 +466,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>50.357539951497323</v>
+        <v>132.21472731702607</v>
       </c>
       <c r="B8">
-        <v>35.960820607690735</v>
+        <v>53.978288755798374</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -477,10 +477,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>54.546543300144471</v>
+        <v>159.5141169572409</v>
       </c>
       <c r="B9">
-        <v>37.317548943874876</v>
+        <v>56.838824487449905</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -488,10 +488,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>58.879476474951218</v>
+        <v>192.29512052321328</v>
       </c>
       <c r="B10">
-        <v>38.654543003430874</v>
+        <v>58.894973353295178</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -499,10 +499,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>63.384097679175881</v>
+        <v>231.88599055908699</v>
       </c>
       <c r="B11">
-        <v>39.976125065687171</v>
+        <v>59.721773696695422</v>
       </c>
       <c r="C11">
         <v>0</v>

</xml_diff>